<commit_message>
Ārpus apdz. vietu kopsavilkuma failā pievienoti visu komponenšu Errors. No mepes izdzēsti lieki faili
</commit_message>
<xml_diff>
--- a/ZPD_Latvija_Arpus_Civilizacijas_Kopsavilkums_Excel.xlsx
+++ b/ZPD_Latvija_Arpus_Civilizacijas_Kopsavilkums_Excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maija Anna Ramāna\Documents\Maija_un_Linda_ZPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D91BFC-7FCA-4AB8-923B-9DAC3B0CEAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABBD8B9-B093-4E91-A0A0-87537EE10398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="97">
   <si>
     <t>GPS N</t>
   </si>
@@ -306,6 +306,24 @@
   </si>
   <si>
     <t>Eksp. mērījumu veikšanas dat.</t>
+  </si>
+  <si>
+    <t>Bx STD</t>
+  </si>
+  <si>
+    <t>By STD</t>
+  </si>
+  <si>
+    <t>Bz STD</t>
+  </si>
+  <si>
+    <t>Bx error</t>
+  </si>
+  <si>
+    <t>By error</t>
+  </si>
+  <si>
+    <t>Bz error</t>
   </si>
 </sst>
 </file>
@@ -3482,16 +3500,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>595195</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>286942</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>86310</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>13803</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>165652</xdr:rowOff>
+      <xdr:colOff>315890</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>79341</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3519,15 +3537,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>597891</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>173</xdr:rowOff>
+      <xdr:colOff>240318</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>61825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>13804</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>41413</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>266571</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>10588</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3872,10 +3890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="103" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3885,7 +3903,7 @@
     <col min="7" max="7" width="25.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3916,8 +3934,26 @@
       <c r="J1" t="s">
         <v>82</v>
       </c>
+      <c r="L1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O1" t="s">
+        <v>91</v>
+      </c>
+      <c r="P1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>57.862904200000003</v>
       </c>
@@ -3948,8 +3984,26 @@
       <c r="J2">
         <v>52011.1</v>
       </c>
+      <c r="L2">
+        <v>1.2303471472024561</v>
+      </c>
+      <c r="M2">
+        <v>0.96249760852452781</v>
+      </c>
+      <c r="N2">
+        <v>0.75302631850449531</v>
+      </c>
+      <c r="O2">
+        <v>143.73488091859826</v>
+      </c>
+      <c r="P2">
+        <v>112.44345098883198</v>
+      </c>
+      <c r="Q2">
+        <v>87.972039814063635</v>
+      </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>57.1404633</v>
       </c>
@@ -3980,8 +4034,26 @@
       <c r="J3">
         <v>51858.2</v>
       </c>
+      <c r="L3">
+        <v>0.63228473095822002</v>
+      </c>
+      <c r="M3">
+        <v>0.74957980295904392</v>
+      </c>
+      <c r="N3">
+        <v>0.80492609956858752</v>
+      </c>
+      <c r="O3">
+        <v>67.138397253790586</v>
+      </c>
+      <c r="P3">
+        <v>79.593234061202992</v>
+      </c>
+      <c r="Q3">
+        <v>85.470114312077172</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>57.706349600000003</v>
       </c>
@@ -4012,8 +4084,26 @@
       <c r="J4">
         <v>51981.4</v>
       </c>
+      <c r="L4">
+        <v>0.62693378268198097</v>
+      </c>
+      <c r="M4">
+        <v>0.27240676173106815</v>
+      </c>
+      <c r="N4">
+        <v>0.71563687811763221</v>
+      </c>
+      <c r="O4">
+        <v>75.900426553744467</v>
+      </c>
+      <c r="P4">
+        <v>32.979223616029522</v>
+      </c>
+      <c r="Q4">
+        <v>86.63936416754126</v>
+      </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>57.613046099999998</v>
       </c>
@@ -4044,8 +4134,26 @@
       <c r="J5">
         <v>51963.4</v>
       </c>
+      <c r="L5">
+        <v>1.1352250317262729</v>
+      </c>
+      <c r="M5">
+        <v>0.97615341563397662</v>
+      </c>
+      <c r="N5">
+        <v>0.90333535191682945</v>
+      </c>
+      <c r="O5">
+        <v>140.12098707882188</v>
+      </c>
+      <c r="P5">
+        <v>120.48675488682916</v>
+      </c>
+      <c r="Q5">
+        <v>111.49881092852904</v>
+      </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>57.465741399999999</v>
       </c>
@@ -4076,8 +4184,26 @@
       <c r="J6">
         <v>51937.3</v>
       </c>
+      <c r="L6">
+        <v>0.6156152455628866</v>
+      </c>
+      <c r="M6">
+        <v>1.3526776234906215</v>
+      </c>
+      <c r="N6">
+        <v>0.734797209996773</v>
+      </c>
+      <c r="O6">
+        <v>67.279733705786526</v>
+      </c>
+      <c r="P6">
+        <v>147.8322555430095</v>
+      </c>
+      <c r="Q6">
+        <v>80.304964785489034</v>
+      </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>57.404880900000002</v>
       </c>
@@ -4108,8 +4234,26 @@
       <c r="J7">
         <v>51925</v>
       </c>
+      <c r="L7">
+        <v>0.62261802504941355</v>
+      </c>
+      <c r="M7">
+        <v>0.33656647938121664</v>
+      </c>
+      <c r="N7">
+        <v>0.69658342722684652</v>
+      </c>
+      <c r="O7">
+        <v>67.993765333437523</v>
+      </c>
+      <c r="P7">
+        <v>36.755155323894584</v>
+      </c>
+      <c r="Q7">
+        <v>76.071247828497903</v>
+      </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>57.3344959</v>
       </c>
@@ -4140,8 +4284,26 @@
       <c r="J8">
         <v>51912.9</v>
       </c>
+      <c r="L8">
+        <v>0.6393485929415561</v>
+      </c>
+      <c r="M8">
+        <v>0.31898794729853674</v>
+      </c>
+      <c r="N8">
+        <v>0.703024193225951</v>
+      </c>
+      <c r="O8">
+        <v>66.933416103826417</v>
+      </c>
+      <c r="P8">
+        <v>33.394854144287038</v>
+      </c>
+      <c r="Q8">
+        <v>73.599615883648141</v>
+      </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>57.287456599999999</v>
       </c>
@@ -4172,8 +4334,26 @@
       <c r="J9">
         <v>51900.7</v>
       </c>
+      <c r="L9">
+        <v>0.63132744384288686</v>
+      </c>
+      <c r="M9">
+        <v>1.5444318399303869</v>
+      </c>
+      <c r="N9">
+        <v>0.91921464451443335</v>
+      </c>
+      <c r="O9">
+        <v>66.929642330013877</v>
+      </c>
+      <c r="P9">
+        <v>163.73162874153533</v>
+      </c>
+      <c r="Q9">
+        <v>97.449759204785209</v>
+      </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>57.223489499999999</v>
       </c>
@@ -4204,8 +4384,26 @@
       <c r="J10">
         <v>51885</v>
       </c>
+      <c r="L10">
+        <v>0.63764837653464124</v>
+      </c>
+      <c r="M10">
+        <v>1.7652044788642125</v>
+      </c>
+      <c r="N10">
+        <v>0.99849452898145585</v>
+      </c>
+      <c r="O10">
+        <v>68.525695007575791</v>
+      </c>
+      <c r="P10">
+        <v>189.69994780200676</v>
+      </c>
+      <c r="Q10">
+        <v>107.30448641861966</v>
+      </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>57.184800899999999</v>
       </c>
@@ -4235,6 +4433,24 @@
       </c>
       <c r="J11">
         <v>51871.199999999997</v>
+      </c>
+      <c r="L11">
+        <v>0.68623044829777413</v>
+      </c>
+      <c r="M11">
+        <v>0.78521469712324965</v>
+      </c>
+      <c r="N11">
+        <v>0.74684855950169626</v>
+      </c>
+      <c r="O11">
+        <v>69.583902808435894</v>
+      </c>
+      <c r="P11">
+        <v>79.620925162840592</v>
+      </c>
+      <c r="Q11">
+        <v>75.730591240736914</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="23">

</xml_diff>

<commit_message>
Pievienoju kļūdas, grafikus ar error bars, jaunos teorētiskos B
</commit_message>
<xml_diff>
--- a/ZPD_Latvija_Arpus_Civilizacijas_Kopsavilkums_Excel.xlsx
+++ b/ZPD_Latvija_Arpus_Civilizacijas_Kopsavilkums_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maija Anna Ramāna\Documents\Maija_un_Linda_ZPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABBD8B9-B093-4E91-A0A0-87537EE10398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD739803-90E1-4834-9109-311A25748E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="99">
   <si>
     <t>GPS N</t>
   </si>
@@ -324,6 +324,12 @@
   </si>
   <si>
     <t>Bz error</t>
+  </si>
+  <si>
+    <t>Propogated SEM</t>
+  </si>
+  <si>
+    <t>Propogated STD</t>
   </si>
 </sst>
 </file>
@@ -663,7 +669,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="lv-LV" baseline="0"/>
-              <a:t> (total) pret GPS N</a:t>
+              <a:t> (total) pret GPS N (Propogated SEM error bars B (total))</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -746,6 +752,123 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Results!$S$2:$S$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>0.93914006025806729</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.75475921243769573</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.3697392207174644</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.9669915910817275</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.273818027393083</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.40700841414346584</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.39853184877337111</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.468697816393352</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.6619340301312502</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.77978507046489676</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Results!$S$2:$S$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>0.93914006025806729</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.75475921243769573</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.3697392207174644</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.9669915910817275</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.273818027393083</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.40700841414346584</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.39853184877337111</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.468697816393352</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.6619340301312502</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.77978507046489676</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Results!$A$2:$A$11</c:f>
@@ -919,34 +1042,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>51998.9</c:v>
+                  <c:v>51999.199999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51845.9</c:v>
+                  <c:v>51846.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>51969.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51950.9</c:v>
+                  <c:v>51951.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51924.800000000003</c:v>
+                  <c:v>51925.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51912.5</c:v>
+                  <c:v>51913</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51900.4</c:v>
+                  <c:v>51901.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51888.2</c:v>
+                  <c:v>51888.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51872.5</c:v>
+                  <c:v>51873.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51858.7</c:v>
+                  <c:v>51859.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -986,6 +1109,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Results!$A$2:$A$11</c:f>
@@ -1032,34 +1169,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>52011.1</c:v>
+                  <c:v>51998.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51858.2</c:v>
+                  <c:v>51845.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51981.4</c:v>
+                  <c:v>51969</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51963.4</c:v>
+                  <c:v>51951.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51937.3</c:v>
+                  <c:v>51924.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>51925</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51912.9</c:v>
+                  <c:v>51900.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51900.7</c:v>
+                  <c:v>51888.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51885</c:v>
+                  <c:v>51872.800000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51871.199999999997</c:v>
+                  <c:v>51858.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1448,7 +1585,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="lv-LV" baseline="0"/>
-              <a:t> (total) pret GPS E</a:t>
+              <a:t> (total) pret GPS E (Propogated SEM error bars for B (total))</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1545,6 +1682,123 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Results!$S$2:$S$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>0.93914006025806729</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.75475921243769573</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.3697392207174644</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.9669915910817275</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.273818027393083</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.40700841414346584</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.39853184877337111</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.468697816393352</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.6619340301312502</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.77978507046489676</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Results!$S$2:$S$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>0.93914006025806729</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.75475921243769573</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.3697392207174644</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.9669915910817275</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.273818027393083</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.40700841414346584</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.39853184877337111</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.468697816393352</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.6619340301312502</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.77978507046489676</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Results!$B$2:$B$11</c:f>
@@ -1718,34 +1972,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>51998.9</c:v>
+                  <c:v>51999.199999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51845.9</c:v>
+                  <c:v>51846.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>51969.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51950.9</c:v>
+                  <c:v>51951.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51924.800000000003</c:v>
+                  <c:v>51925.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51912.5</c:v>
+                  <c:v>51913</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51900.4</c:v>
+                  <c:v>51901.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51888.2</c:v>
+                  <c:v>51888.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51872.5</c:v>
+                  <c:v>51873.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51858.7</c:v>
+                  <c:v>51859.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1845,34 +2099,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>52011.1</c:v>
+                  <c:v>51998.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51858.2</c:v>
+                  <c:v>51845.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51981.4</c:v>
+                  <c:v>51969</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51963.4</c:v>
+                  <c:v>51951.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51937.3</c:v>
+                  <c:v>51924.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>51925</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51912.9</c:v>
+                  <c:v>51900.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51900.7</c:v>
+                  <c:v>51888.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51885</c:v>
+                  <c:v>51872.800000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51871.199999999997</c:v>
+                  <c:v>51858.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2260,6 +2514,1943 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="lv-LV" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>B (total) pret GPS N (Propogated STD error bars for B (total))</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>B (total) eksperimentālais</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Results!$T$2:$T$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>109.71471347254329</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>80.143203456463851</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>44.762884600111057</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>119.35590957966394</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>139.21379999982838</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>44.447853236836572</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>41.722306671305496</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>155.70275061025606</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>178.60185748516264</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>79.070359948752355</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Results!$T$2:$T$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>109.71471347254329</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>80.143203456463851</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>44.762884600111057</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>119.35590957966394</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>139.21379999982838</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>44.447853236836572</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>41.722306671305496</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>155.70275061025606</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>178.60185748516264</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>79.070359948752355</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>57.862904200000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.1404633</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.706349600000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57.613046099999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.465741399999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.404880900000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57.3344959</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57.287456599999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57.223489499999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>57.184800899999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>54814.980689999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53311.06237</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54739.182419999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53959.366909999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54311.215179999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53686.451399999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53675.088889999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53491.282509999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53488.626629999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52776.948049999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-995C-4F43-AE4F-50794155882A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>B (total) teorētiskais 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>57.862904200000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.1404633</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.706349600000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57.613046099999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.465741399999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.404880900000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57.3344959</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57.287456599999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57.223489499999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>57.184800899999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$I$2:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>51999.199999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51846.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51969.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51951.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51925.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51913</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51901.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51888.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51873.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51859.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-995C-4F43-AE4F-50794155882A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>B (total) teorētiskais 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>57.862904200000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.1404633</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.706349600000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57.613046099999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.465741399999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.404880900000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57.3344959</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57.287456599999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57.223489499999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>57.184800899999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$J$2:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>51998.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51845.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51969</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51951.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51924.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51925</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51900.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51888.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51872.800000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51858.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-995C-4F43-AE4F-50794155882A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="112128304"/>
+        <c:axId val="112123984"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="112128304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="lv-LV" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>GPS N (°)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="112123984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="112123984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="lv-LV"/>
+                  <a:t>B</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="lv-LV" baseline="0"/>
+                  <a:t> (Total) (nT)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="112128304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="lv-LV" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>B (total) pret GPS E (Propogated STD error bars for B (total))</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>B (total) eksperimentālais</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Results!$T$2:$T$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>109.71471347254329</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>80.143203456463851</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>44.762884600111057</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>119.35590957966394</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>139.21379999982838</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>44.447853236836572</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>41.722306671305496</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>155.70275061025606</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>178.60185748516264</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>79.070359948752355</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Results!$T$2:$T$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>109.71471347254329</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>80.143203456463851</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>44.762884600111057</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>119.35590957966394</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>139.21379999982838</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>44.447853236836572</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>41.722306671305496</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>155.70275061025606</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>178.60185748516264</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>79.070359948752355</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>24.352066300000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.290671199999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.375397499999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.3862953</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.431335000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.433516300000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.4600957</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.430827099999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.401625500000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.334432799999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>54814.980689999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53311.06237</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54739.182419999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53959.366909999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54311.215179999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53686.451399999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53675.088889999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53491.282509999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53488.626629999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52776.948049999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E137-4BC9-B018-361820D8E337}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>B (total) teorētiskais 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>24.352066300000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.290671199999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.375397499999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.3862953</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.431335000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.433516300000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.4600957</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.430827099999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.401625500000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.334432799999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$I$2:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>51999.199999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51846.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51969.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51951.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51925.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51913</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51901.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51888.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51873.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51859.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E137-4BC9-B018-361820D8E337}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>B (total) teorētiskais 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>24.352066300000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.290671199999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.375397499999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.3862953</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.431335000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.433516300000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.4600957</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.430827099999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.401625500000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.334432799999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$J$2:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>51998.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51845.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51969</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51951.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51924.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51925</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51900.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51888.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51872.800000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51858.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E137-4BC9-B018-361820D8E337}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="297869472"/>
+        <c:axId val="297871392"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="297869472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="lv-LV"/>
+                  <a:t>GPS E </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="lv-LV" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>(°)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="297871392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="297871392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="lv-LV" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>B (total) (nT)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="297869472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2340,6 +4531,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2857,6 +5128,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3500,16 +6803,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>286942</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>86310</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>141796</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>315890</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>79341</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1150987</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>17691</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3536,16 +6839,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>240318</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>61825</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>490856</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>108334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>266571</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>10588</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>578733</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>8038</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3565,6 +6868,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1160154</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>108729</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>467894</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>289648</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5637E8A8-1530-C40E-1DB1-C799688813FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>600806</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>123091</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>498231</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>166076</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{788A1EA9-6FCC-2EDB-2E7B-8EFDC425E26B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3890,10 +7265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="K5" zoomScale="90" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3901,9 +7276,11 @@
     <col min="2" max="2" width="11.81640625" customWidth="1"/>
     <col min="3" max="3" width="15.81640625" customWidth="1"/>
     <col min="7" max="7" width="25.26953125" customWidth="1"/>
+    <col min="19" max="19" width="14.453125" customWidth="1"/>
+    <col min="20" max="20" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3952,8 +7329,14 @@
       <c r="Q1" t="s">
         <v>93</v>
       </c>
+      <c r="S1" t="s">
+        <v>97</v>
+      </c>
+      <c r="T1" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:20">
       <c r="A2">
         <v>57.862904200000003</v>
       </c>
@@ -3976,13 +7359,13 @@
         <v>84</v>
       </c>
       <c r="H2">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="I2">
-        <v>51998.9</v>
+        <v>51999.199999999997</v>
       </c>
       <c r="J2">
-        <v>52011.1</v>
+        <v>51998.8</v>
       </c>
       <c r="L2">
         <v>1.2303471472024561</v>
@@ -4002,8 +7385,16 @@
       <c r="Q2">
         <v>87.972039814063635</v>
       </c>
+      <c r="S2">
+        <f>SQRT((D2/C2*L2)^2 + (E2/C2*M2)^2 + (F2/C2*N2)^2)</f>
+        <v>0.93914006025806729</v>
+      </c>
+      <c r="T2">
+        <f>SQRT((D2/C2*O2)^2 + (E2/C2*P2)^2 + (F2/C2*Q2)^2)</f>
+        <v>109.71471347254329</v>
+      </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:20">
       <c r="A3">
         <v>57.1404633</v>
       </c>
@@ -4026,13 +7417,13 @@
         <v>84</v>
       </c>
       <c r="H3">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="I3">
-        <v>51845.9</v>
+        <v>51846.3</v>
       </c>
       <c r="J3">
-        <v>51858.2</v>
+        <v>51845.8</v>
       </c>
       <c r="L3">
         <v>0.63228473095822002</v>
@@ -4052,8 +7443,16 @@
       <c r="Q3">
         <v>85.470114312077172</v>
       </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S11" si="0">SQRT((D3/C3*L3)^2 + (E3/C3*M3)^2 + (F3/C3*N3)^2)</f>
+        <v>0.75475921243769573</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T11" si="1">SQRT((D3/C3*O3)^2 + (E3/C3*P3)^2 + (F3/C3*Q3)^2)</f>
+        <v>80.143203456463851</v>
+      </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:20">
       <c r="A4">
         <v>57.706349600000003</v>
       </c>
@@ -4076,13 +7475,13 @@
         <v>84</v>
       </c>
       <c r="H4">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="I4">
         <v>51969.1</v>
       </c>
       <c r="J4">
-        <v>51981.4</v>
+        <v>51969</v>
       </c>
       <c r="L4">
         <v>0.62693378268198097</v>
@@ -4102,8 +7501,16 @@
       <c r="Q4">
         <v>86.63936416754126</v>
       </c>
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>0.3697392207174644</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="1"/>
+        <v>44.762884600111057</v>
+      </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:20">
       <c r="A5">
         <v>57.613046099999998</v>
       </c>
@@ -4126,13 +7533,13 @@
         <v>84</v>
       </c>
       <c r="H5">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>51950.9</v>
+        <v>51951.8</v>
       </c>
       <c r="J5">
-        <v>51963.4</v>
+        <v>51951.3</v>
       </c>
       <c r="L5">
         <v>1.1352250317262729</v>
@@ -4152,8 +7559,16 @@
       <c r="Q5">
         <v>111.49881092852904</v>
       </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>0.9669915910817275</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="1"/>
+        <v>119.35590957966394</v>
+      </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:20">
       <c r="A6">
         <v>57.465741399999999</v>
       </c>
@@ -4176,13 +7591,13 @@
         <v>84</v>
       </c>
       <c r="H6">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="I6">
-        <v>51924.800000000003</v>
+        <v>51925.3</v>
       </c>
       <c r="J6">
-        <v>51937.3</v>
+        <v>51924.9</v>
       </c>
       <c r="L6">
         <v>0.6156152455628866</v>
@@ -4202,8 +7617,16 @@
       <c r="Q6">
         <v>80.304964785489034</v>
       </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>1.273818027393083</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="1"/>
+        <v>139.21379999982838</v>
+      </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:20">
       <c r="A7">
         <v>57.404880900000002</v>
       </c>
@@ -4226,10 +7649,10 @@
         <v>84</v>
       </c>
       <c r="H7">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="I7">
-        <v>51912.5</v>
+        <v>51913</v>
       </c>
       <c r="J7">
         <v>51925</v>
@@ -4252,8 +7675,16 @@
       <c r="Q7">
         <v>76.071247828497903</v>
       </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>0.40700841414346584</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="1"/>
+        <v>44.447853236836572</v>
+      </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:20">
       <c r="A8">
         <v>57.3344959</v>
       </c>
@@ -4276,13 +7707,13 @@
         <v>85</v>
       </c>
       <c r="H8">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="I8">
-        <v>51900.4</v>
+        <v>51901.1</v>
       </c>
       <c r="J8">
-        <v>51912.9</v>
+        <v>51900.7</v>
       </c>
       <c r="L8">
         <v>0.6393485929415561</v>
@@ -4302,8 +7733,16 @@
       <c r="Q8">
         <v>73.599615883648141</v>
       </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>0.39853184877337111</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>41.722306671305496</v>
+      </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:20">
       <c r="A9">
         <v>57.287456599999999</v>
       </c>
@@ -4326,13 +7765,13 @@
         <v>85</v>
       </c>
       <c r="H9">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="I9">
-        <v>51888.2</v>
+        <v>51888.9</v>
       </c>
       <c r="J9">
-        <v>51900.7</v>
+        <v>51888.5</v>
       </c>
       <c r="L9">
         <v>0.63132744384288686</v>
@@ -4352,8 +7791,16 @@
       <c r="Q9">
         <v>97.449759204785209</v>
       </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>1.468697816393352</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="1"/>
+        <v>155.70275061025606</v>
+      </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:20">
       <c r="A10">
         <v>57.223489499999999</v>
       </c>
@@ -4376,13 +7823,13 @@
         <v>85</v>
       </c>
       <c r="H10">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="I10">
-        <v>51872.5</v>
+        <v>51873.2</v>
       </c>
       <c r="J10">
-        <v>51885</v>
+        <v>51872.800000000003</v>
       </c>
       <c r="L10">
         <v>0.63764837653464124</v>
@@ -4402,8 +7849,16 @@
       <c r="Q10">
         <v>107.30448641861966</v>
       </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>1.6619340301312502</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="1"/>
+        <v>178.60185748516264</v>
+      </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:20">
       <c r="A11">
         <v>57.184800899999999</v>
       </c>
@@ -4426,13 +7881,13 @@
         <v>85</v>
       </c>
       <c r="H11">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="I11">
-        <v>51858.7</v>
+        <v>51859.4</v>
       </c>
       <c r="J11">
-        <v>51871.199999999997</v>
+        <v>51858.9</v>
       </c>
       <c r="L11">
         <v>0.68623044829777413</v>
@@ -4451,6 +7906,14 @@
       </c>
       <c r="Q11">
         <v>75.730591240736914</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="0"/>
+        <v>0.77978507046489676</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>79.070359948752355</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="23">

</xml_diff>